<commit_message>
Updated planning documents (sprint 2 report)
</commit_message>
<xml_diff>
--- a/Planning_Documents/sprint_2/sprint 2 burnup.xlsx
+++ b/Planning_Documents/sprint_2/sprint 2 burnup.xlsx
@@ -167,11 +167,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1928742832"/>
-        <c:axId val="248106762"/>
+        <c:axId val="1048517394"/>
+        <c:axId val="1786554128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1928742832"/>
+        <c:axId val="1048517394"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -203,10 +203,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="248106762"/>
+        <c:crossAx val="1786554128"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="248106762"/>
+        <c:axId val="1786554128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -254,18 +254,19 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1928742832"/>
+        <c:crossAx val="1048517394"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:overlay val="0"/>
     </c:legend>
+    <c:plotVisOnly val="1"/>
   </c:chart>
 </c:chartSpace>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -400,7 +401,7 @@
         <v>42787.0</v>
       </c>
       <c r="B9" s="3">
-        <v>26.0</v>
+        <v>40.0</v>
       </c>
       <c r="C9" s="3">
         <v>65.0</v>
@@ -411,7 +412,7 @@
         <v>42788.0</v>
       </c>
       <c r="B10" s="3">
-        <v>0.0</v>
+        <v>42.0</v>
       </c>
       <c r="C10" s="3">
         <v>65.0</v>
@@ -422,7 +423,7 @@
         <v>42789.0</v>
       </c>
       <c r="B11" s="3">
-        <v>0.0</v>
+        <v>48.0</v>
       </c>
       <c r="C11" s="3">
         <v>65.0</v>
@@ -433,7 +434,7 @@
         <v>42790.0</v>
       </c>
       <c r="B12" s="3">
-        <v>0.0</v>
+        <v>48.5</v>
       </c>
       <c r="C12" s="3">
         <v>65.0</v>
@@ -444,7 +445,7 @@
         <v>42791.0</v>
       </c>
       <c r="B13" s="3">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C13" s="3">
         <v>65.0</v>
@@ -455,7 +456,7 @@
         <v>42792.0</v>
       </c>
       <c r="B14" s="3">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C14" s="3">
         <v>65.0</v>
@@ -466,7 +467,7 @@
         <v>42793.0</v>
       </c>
       <c r="B15" s="3">
-        <v>0.0</v>
+        <v>51.0</v>
       </c>
       <c r="C15" s="3">
         <v>65.0</v>
@@ -477,7 +478,7 @@
         <v>42794.0</v>
       </c>
       <c r="B16" s="3">
-        <v>0.0</v>
+        <v>59.0</v>
       </c>
       <c r="C16" s="3">
         <v>65.0</v>

</xml_diff>